<commit_message>
commit message 2 because previous push didnt work
</commit_message>
<xml_diff>
--- a/Employee.xlsx
+++ b/Employee.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c21ddadc23376b4d/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zapca\Downloads\Flask-Bootcamp-master\Flask-Bootcamp-master\Capstone1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6B5E4474-1F6E-4159-B7F4-6D6BF1D72323}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{109C77A2-D251-42D7-ABB1-0C06E59B0B5C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{8B3CF5CE-56A9-49A6-98A1-37FAE77AC01D}"/>
   </bookViews>

</xml_diff>